<commit_message>
trying to fix no airports
</commit_message>
<xml_diff>
--- a/Web/airport_to_city_map.xlsx
+++ b/Web/airport_to_city_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\UT Austin 2015 Fall\Projects\JetBlue\Web\jetblue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\UT Austin 2015 Fall\Projects\JetBlue\Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="396">
   <si>
     <t>BHM</t>
   </si>
@@ -1110,6 +1110,108 @@
   </si>
   <si>
     <t>Rock Springs Wyoming</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Cancun</t>
+  </si>
+  <si>
+    <t>Saint Maarten</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Providenciales</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>SJU</t>
+  </si>
+  <si>
+    <t>BGI</t>
+  </si>
+  <si>
+    <t>SDQ</t>
+  </si>
+  <si>
+    <t>CUN</t>
+  </si>
+  <si>
+    <t>SXM</t>
+  </si>
+  <si>
+    <t>AUA</t>
+  </si>
+  <si>
+    <t>UVF</t>
+  </si>
+  <si>
+    <t>NAS</t>
+  </si>
+  <si>
+    <t>CUR</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>MBJ</t>
+  </si>
+  <si>
+    <t>LIR</t>
+  </si>
+  <si>
+    <t>BDA</t>
+  </si>
+  <si>
+    <t>GCM</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>PUJ</t>
+  </si>
+  <si>
+    <t>AZS</t>
+  </si>
+  <si>
+    <t>LRM</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,6 +3033,158 @@
         <v>361</v>
       </c>
     </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>377</v>
+      </c>
+      <c r="B188" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>378</v>
+      </c>
+      <c r="B189" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>379</v>
+      </c>
+      <c r="B190" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>381</v>
+      </c>
+      <c r="B192" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>382</v>
+      </c>
+      <c r="B193" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>383</v>
+      </c>
+      <c r="B194" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>384</v>
+      </c>
+      <c r="B195" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>385</v>
+      </c>
+      <c r="B196" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>386</v>
+      </c>
+      <c r="B197" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>387</v>
+      </c>
+      <c r="B198" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>388</v>
+      </c>
+      <c r="B199" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>389</v>
+      </c>
+      <c r="B200" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>390</v>
+      </c>
+      <c r="B201" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>391</v>
+      </c>
+      <c r="B202" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>392</v>
+      </c>
+      <c r="B203" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>393</v>
+      </c>
+      <c r="B204" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>394</v>
+      </c>
+      <c r="B205" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>395</v>
+      </c>
+      <c r="B206" t="s">
+        <v>364</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>